<commit_message>
created logic for check price of tractor.
</commit_message>
<xml_diff>
--- a/Content/FarmImplements/FarmImplements/Implement.xlsx
+++ b/Content/FarmImplements/FarmImplements/Implement.xlsx
@@ -14,30 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
-  <si>
-    <t>Haritdisha</t>
-  </si>
-  <si>
-    <t>Balwaan</t>
-  </si>
-  <si>
-    <t>MINI HD200-DRG-FX</t>
-  </si>
-  <si>
-    <t>BS-22</t>
-  </si>
-  <si>
-    <t>BS-21</t>
-  </si>
-  <si>
-    <t>['MINIHD200-DRG-FXimg0-mini-hd200-drg-fx-56-1688626341.png', 'MINIHD200-DRG-FXimg1-default-image.png', 'MINIHD200-DRG-FXimg2-mini-hd200-drg-fx-56-1688626341.png']</t>
-  </si>
-  <si>
-    <t>['BS-22img0-bs-22-56-1686815024.png', 'BS-22img1-default-image.png', 'BS-22img2-bs-22-56-1686815024.png']</t>
-  </si>
-  <si>
-    <t>['BS-21img0-bs-21-56-1686814739.png', 'BS-21img1-default-image.png', 'BS-21img2-bs-21-56-1686814739.png']</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>Neptune</t>
+  </si>
+  <si>
+    <t>PS-50 Power</t>
+  </si>
+  <si>
+    <t>NF-10B Manual</t>
+  </si>
+  <si>
+    <t>['PS-50Powerimg0-ps-50-power-56-1650083453.png', 'PS-50Powerimg1-default-image.png', 'PS-50Powerimg2-ps-50-power-56-1650083453.png']</t>
+  </si>
+  <si>
+    <t>['NF-10BManualimg0-nf-10b-manual-56-1650083150.png', 'NF-10BManualimg1-default-image.png', 'NF-10BManualimg2-nf-10b-manual-56-1650083150.png']</t>
   </si>
   <si>
     <t>product</t>
@@ -408,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -416,16 +407,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -433,41 +424,27 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>